<commit_message>
Updated WTI time series
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[0.9999999999999999, 0.287234352583415, 0.23852061621122886, 0.19245267592210355, 0.23472661705860698, 0.4116760149571437, 0.24559714732360596, 0.2508907632633834, 0.22417730180293083, 0.19528300635570905, 0.19171063593340967, 0.17170326977157493, 0.2256120278219933, 0.2148992175179589, 0.21797339306782346, 0.20657162708835314, 0.18009837577302576, 0.1636676262426473, 0.1839118842223335, 0.1872437878609929]</t>
+    <t>[1.0, 0.26849639589116786, 0.22505312456727433, 0.18086882463235954, 0.21866088844794498, 0.412253415377217, 0.23574147422888128, 0.23024994926453998, 0.2076300442004622, 0.18610908150066174, 0.18823133562378067, 0.16510421240250717, 0.20856794520950364, 0.1974727474168753, 0.20848744708967146, 0.19630366308928024, 0.16955177400282306, 0.15325287159781073, 0.17051581590452933, 0.18293849936896858]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.27564588438814075, 0.27341117378221264, 0.23972925321371608, 0.237913635639217, 0.2812670119817782, 0.2126282469826813, 0.2046732468476288, 0.19321475343845348, 0.17879671779744682, 0.20253048118351916, 0.17683098326677935, 0.2085261786578687, 0.18525086597550258, 0.1893840872826723, 0.18390715309260944, 0.18699591535909083, 0.18225376998394113, 0.19113591084570558, 0.1683205024396686]</t>
+    <t>[1.0, 0.25884637756886275, 0.2617487846700429, 0.22993176870304186, 0.220724096060218, 0.26978210485776444, 0.20788333748641685, 0.1936046509572187, 0.18306401893496915, 0.17758361340898515, 0.19762017844058155, 0.17638647416796083, 0.1941811472603485, 0.17199519518040712, 0.17472908300306267, 0.16966178231567364, 0.1752614753527359, 0.17180103759771792, 0.17648721296334924, 0.15890376522321634]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.011174726661797245, -0.022132056811053704, -0.06677686046627598, -0.07247548449874769, 0.2883137005728095, 0.010841328527603755, 0.04252125301696295, 0.00493972649427982, -0.03395228239297903, -0.03661777784604101, -0.06436857597989706, -0.006608010094395917, 0.0016120552871589273, 0.022747469263519112, 0.023888612781097454, -0.02010327992124273, -0.05114646553555743, -0.065338631176492, -0.013476269203422507]</t>
+    <t>[1.0, 0.008867132856130135, -0.023230276341758796, -0.06926220255770238, -0.07285238917724701, 0.2979272459621906, 0.005589135549483667, 0.04217071579404857, 0.007453349983234831, -0.03471032298363181, -0.029098854219604803, -0.06536773871805338, -0.005223547281206571, 0.002819427011188702, 0.026292303157612742, 0.023052660445758197, -0.01675903194166831, -0.05160411480126559, -0.06570039991303565, -0.010805284262188254]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[0.9999999999999998, 0.00994899059244851, -0.023334882337666965, -0.06776165066391952, -0.07316773551874399, 0.2881448515404446, 0.01022992540138105, 0.04165155384633442, 0.004300603125061676, -0.034386493914457986, -0.03714312808642545, -0.06443248923023598, -0.007113646307139469, 0.0008553658152078553, 0.02180315581635161, 0.02318902761885157, -0.02026290539381402, -0.051098709849133055, -0.06558967672114675, -0.013619127616073505]</t>
-  </si>
-  <si>
-    <t>[1.0, 0.031682606957506604, -0.0026550814147308665, -0.03658771949507313, -0.034019168607542435, 0.2284378032487314, -0.016466636161093073, 0.027976325407632997, 0.0011450477539569593, -0.04218866013606649, -0.025148134587155622, -0.05195612850754465, -0.0003541427673329583, 0.004948266657316484, 0.0099774801885729, 0.022725985409667002, -0.02257609656516505, -0.045668104714449, -0.037961333218374284, -0.015043199003039371]</t>
+    <t>[1.0, 0.001459771354261513, -0.029077623349178607, -0.07551332924127507, -0.07798047635072364, 0.29344027645172804, 0.002631354327241632, 0.03825618307539085, 0.0038356249194194726, -0.03505159419641644, -0.031005892758576094, -0.06558006423733534, -0.005311623535753787, 0.0013744475394346918, 0.026481216283841723, 0.023613476435799776, -0.014959483618344723, -0.04930850137756249, -0.06320848916305259, -0.008963607381714329]</t>
+  </si>
+  <si>
+    <t>[1.0, 0.020910474950645016, -0.006627601430572927, -0.04043897220385024, -0.0405359872024497, 0.23173505625960134, -0.018088443182852996, 0.02101201353600799, -0.003675837270166394, -0.0414038404034892, -0.01335152439385969, -0.04742806255177747, 0.0015548257082108768, 0.002497137695331543, 0.011495571759409852, 0.020972810071177444, -0.018452329860599446, -0.04143314346947491, -0.03559735364959534, -0.011639602172060509]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.001741393671579251</v>
+        <v>0.0003357362608120886</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7813996980498726</v>
+        <v>0.7811066170815903</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1090195833329348</v>
+        <v>0.1096168593744059</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8847643641058748</v>
+        <v>0.8985549132947976</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.113163749114964</v>
+        <v>-0.1163566168657372</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.7181891053505461</v>
+        <v>0.7143333191914079</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.07741914748519928</v>
+        <v>0.07857022141353169</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.1298768193474663</v>
+        <v>0.127493519308936</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.6491751979809366</v>
+        <v>0.6537753089210313</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.0617326657432364</v>
+        <v>0.06026787667470801</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.0003740109087404437</v>
+        <v>-0.0003275855018089072</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0003749290372394447</v>
+        <v>0.0004546839189019739</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05202964205909438</v>
+        <v>0.05441414546162113</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9458356166642519</v>
+        <v>0.9433684781935523</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.001787104101385869</v>
+        <v>-0.002287620620664199</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0003746363834588962</v>
+        <v>0.0009722529880505443</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04531781678990217</v>
+        <v>0.05203551811178871</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9447831199734813</v>
+        <v>0.9263793368439823</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.01581598172098774</v>
+        <v>0.02638316736636755</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.003637835604587994</v>
+        <v>0.003031682556865371</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0003029989307433213</v>
+        <v>0.0008397951808298639</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.03977576676231637</v>
+        <v>0.0444361120918518</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9494222433530769</v>
+        <v>0.9337842325354975</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.01721394194083427</v>
+        <v>0.028719871382662</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7873936273700367</v>
+        <v>0.7852304668220104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized definition of virtual environment
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[1.0, 0.26849639589116786, 0.22505312456727433, 0.18086882463235954, 0.21866088844794498, 0.412253415377217, 0.23574147422888128, 0.23024994926453998, 0.2076300442004622, 0.18610908150066174, 0.18823133562378067, 0.16510421240250717, 0.20856794520950364, 0.1974727474168753, 0.20848744708967146, 0.19630366308928024, 0.16955177400282306, 0.15325287159781073, 0.17051581590452933, 0.18293849936896858]</t>
+    <t>[0.9999999999999999, 0.2848119991792331, 0.2334356714793047, 0.1884336348211745, 0.23232495920002785, 0.4084685571727982, 0.24390892954114599, 0.24637731116838943, 0.2195950669032209, 0.19049379276934764, 0.18844228261075033, 0.168744803484475, 0.2220131456710551, 0.20815171860752224, 0.2130526454436412, 0.20095992871290813, 0.17677001340986137, 0.15930317633191526, 0.1790359238292295, 0.18302755053862838]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.25884637756886275, 0.2617487846700429, 0.22993176870304186, 0.220724096060218, 0.26978210485776444, 0.20788333748641685, 0.1936046509572187, 0.18306401893496915, 0.17758361340898515, 0.19762017844058155, 0.17638647416796083, 0.1941811472603485, 0.17199519518040712, 0.17472908300306267, 0.16966178231567364, 0.1752614753527359, 0.17180103759771792, 0.17648721296334924, 0.15890376522321634]</t>
+    <t>[1.0, 0.2709540677350821, 0.26721990309133725, 0.23072343204292584, 0.22874811051070423, 0.27251636979825433, 0.20516276535812522, 0.19685093437325013, 0.18630407918150968, 0.17245986290762602, 0.19478444685645047, 0.16961726962247356, 0.2011101630896298, 0.17966326359570117, 0.1823651825479308, 0.17906681112390138, 0.1798760075404138, 0.17708847267990474, 0.18537518343687875, 0.16282967064087508]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.008867132856130135, -0.023230276341758796, -0.06926220255770238, -0.07285238917724701, 0.2979272459621906, 0.005589135549483667, 0.04217071579404857, 0.007453349983234831, -0.03471032298363181, -0.029098854219604803, -0.06536773871805338, -0.005223547281206571, 0.002819427011188702, 0.026292303157612742, 0.023052660445758197, -0.01675903194166831, -0.05160411480126559, -0.06570039991303565, -0.010805284262188254]</t>
+    <t>[1.0, 0.012921484748652453, -0.026072343461510026, -0.06395318896691948, -0.07457061134478891, 0.28415198586866247, 0.011226160866768017, 0.042061986071826055, 0.0074122145730563015, -0.035960630026002874, -0.03897814043332797, -0.058845018297552946, -0.008157874727687857, -0.008459946571520601, 0.022237295878262855, 0.019433928941365638, -0.017960817765663915, -0.04639642287492738, -0.07529952439314666, -0.012642632212823347]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.001459771354261513, -0.029077623349178607, -0.07551332924127507, -0.07798047635072364, 0.29344027645172804, 0.002631354327241632, 0.03825618307539085, 0.0038356249194194726, -0.03505159419641644, -0.031005892758576094, -0.06558006423733534, -0.005311623535753787, 0.0013744475394346918, 0.026481216283841723, 0.023613476435799776, -0.014959483618344723, -0.04930850137756249, -0.06320848916305259, -0.008963607381714329]</t>
-  </si>
-  <si>
-    <t>[1.0, 0.020910474950645016, -0.006627601430572927, -0.04043897220385024, -0.0405359872024497, 0.23173505625960134, -0.018088443182852996, 0.02101201353600799, -0.003675837270166394, -0.0414038404034892, -0.01335152439385969, -0.04742806255177747, 0.0015548257082108768, 0.002497137695331543, 0.011495571759409852, 0.020972810071177444, -0.018452329860599446, -0.04143314346947491, -0.03559735364959534, -0.011639602172060509]</t>
+    <t>[1.0, 0.01170640069309429, -0.027019871792121383, -0.06473556769136818, -0.07523460134067694, 0.28394915683882177, 0.010571844304318033, 0.04139500528711297, 0.006843809719162673, -0.036535031037552776, -0.03956013651383042, -0.05902292178768356, -0.008589463593761677, -0.008996289543797251, 0.02123524169535309, 0.018803478144489818, -0.01825499053900965, -0.04635009855593515, -0.07558730364559292, -0.012818501239923279]</t>
+  </si>
+  <si>
+    <t>[0.9999999999999998, 0.03436747043835898, -0.009916977392808952, -0.036342088441116874, -0.03398037899371765, 0.2278832559768839, -0.015526867512406386, 0.024832353317328033, -0.0012328249086491533, -0.04742429740295087, -0.021595739425330534, -0.049224940512919396, -0.0010460084428602415, -0.006020314176895672, 0.007707317433711263, 0.02113771040858326, -0.019646713496766777, -0.04458143120438001, -0.04379339936949635, -0.014302923625889639]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.0003357362608120886</v>
+        <v>0.000938174311667381</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7811066170815903</v>
+        <v>0.7809438713439286</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1096168593744059</v>
+        <v>0.1183709823931952</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8985549132947976</v>
+        <v>0.8918518518518519</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1163566168657372</v>
+        <v>-0.1201920800837948</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.7143333191914079</v>
+        <v>0.7146600096275811</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.07857022141353169</v>
+        <v>0.08437256151599415</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.127493519308936</v>
+        <v>0.135949515535049</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.6537753089210313</v>
+        <v>0.6457680558412187</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.06026787667470801</v>
+        <v>0.06696972555906473</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.0003275855018089072</v>
+        <v>-0.0004208491891122551</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0004546839189019739</v>
+        <v>0.0003309222042712687</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05441414546162113</v>
+        <v>0.05181414205162736</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9433684781935523</v>
+        <v>0.9470128795253214</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.002287620620664199</v>
+        <v>-0.001562538384524367</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0009722529880505443</v>
+        <v>0.0003317251781729857</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05203551811178871</v>
+        <v>0.04650875848957307</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9263793368439823</v>
+        <v>0.946142285572969</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.02638316736636755</v>
+        <v>0.0125454530356663</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.003031682556865371</v>
+        <v>0.00319136883951554</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0008397951808298639</v>
+        <v>0.0002683582271512838</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.0444361120918518</v>
+        <v>0.04218000568309339</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9337842325354975</v>
+        <v>0.9502592922823111</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.028719871382662</v>
+        <v>0.01257965920255122</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7852304668220104</v>
+        <v>0.7871140150637183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunti file con considerazioni su calcolo lambda; aggiornate stime con std moving average
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[0.9999999999999999, 0.2848119991792331, 0.2334356714793047, 0.1884336348211745, 0.23232495920002785, 0.4084685571727982, 0.24390892954114599, 0.24637731116838943, 0.2195950669032209, 0.19049379276934764, 0.18844228261075033, 0.168744803484475, 0.2220131456710551, 0.20815171860752224, 0.2130526454436412, 0.20095992871290813, 0.17677001340986137, 0.15930317633191526, 0.1790359238292295, 0.18302755053862838]</t>
+    <t>[1.0, 0.020742072449138466, -0.046057578182718904, -0.09987740779527826, -0.11362098275977535, 0.07053872377467447, 0.027242553341174296, 0.038508958376020745, 0.022524839067012383, -0.014046769068594755, -0.041041619122136656, -0.030166978710828258, -0.0071719504665959215, 0.05899539513191117, 0.05611133351917008, 0.03036155380748464, -0.006839678743164695, -0.03382079672006651, -0.04097821460225061, 0.002374139634956119]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.2709540677350821, 0.26721990309133725, 0.23072343204292584, 0.22874811051070423, 0.27251636979825433, 0.20516276535812522, 0.19685093437325013, 0.18630407918150968, 0.17245986290762602, 0.19478444685645047, 0.16961726962247356, 0.2011101630896298, 0.17966326359570117, 0.1823651825479308, 0.17906681112390138, 0.1798760075404138, 0.17708847267990474, 0.18537518343687875, 0.16282967064087508]</t>
+    <t>[1.0, 0.059786836446393266, 0.008164407218926334, -0.0022021570605025636, -0.00600966558310538, 0.010383753667678432, 0.016637941679735126, -0.02002175112349545, 0.00828413956072075, -0.008164560034633245, 0.012766997876978145, 0.018733138120191988, 0.013428564824778264, 0.029600391644876812, 0.019874002882877304, -4.271655568156782e-05, -0.015510411516043895, -0.007215655497153533, -0.004023081281778683, -0.012554653841117053]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.012921484748652453, -0.026072343461510026, -0.06395318896691948, -0.07457061134478891, 0.28415198586866247, 0.011226160866768017, 0.042061986071826055, 0.0074122145730563015, -0.035960630026002874, -0.03897814043332797, -0.058845018297552946, -0.008157874727687857, -0.008459946571520601, 0.022237295878262855, 0.019433928941365638, -0.017960817765663915, -0.04639642287492738, -0.07529952439314666, -0.012642632212823347]</t>
+    <t>[1.0, 0.0046055459593722405, -0.03433958921631113, -0.09108536610602833, -0.13236200747524696, 0.09214281163745758, 0.05071434479689837, 0.04263232309750947, 0.03213706187886878, 8.049679111961297e-05, -0.053645870199857094, -0.025443903188358093, -0.010255174641980542, 0.05561505926299536, 0.04912782792613663, 0.018314890859462658, -0.0050686743117231165, -0.0302937502907785, -0.05743611288880337, -0.0029958877751506195]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.01170640069309429, -0.027019871792121383, -0.06473556769136818, -0.07523460134067694, 0.28394915683882177, 0.010571844304318033, 0.04139500528711297, 0.006843809719162673, -0.036535031037552776, -0.03956013651383042, -0.05902292178768356, -0.008589463593761677, -0.008996289543797251, 0.02123524169535309, 0.018803478144489818, -0.01825499053900965, -0.04635009855593515, -0.07558730364559292, -0.012818501239923279]</t>
-  </si>
-  <si>
-    <t>[0.9999999999999998, 0.03436747043835898, -0.009916977392808952, -0.036342088441116874, -0.03398037899371765, 0.2278832559768839, -0.015526867512406386, 0.024832353317328033, -0.0012328249086491533, -0.04742429740295087, -0.021595739425330534, -0.049224940512919396, -0.0010460084428602415, -0.006020314176895672, 0.007707317433711263, 0.02113771040858326, -0.019646713496766777, -0.04458143120438001, -0.04379339936949635, -0.014302923625889639]</t>
+    <t>[1.0, 0.0029458747712240037, -0.034465194544982605, -0.09075287544891736, -0.13238801623191018, 0.09284870902027942, 0.050533654351551584, 0.041719372478274556, 0.03344411420821392, 0.00010641221794151788, -0.05233931341253185, -0.025471747071868847, -0.01021390984255276, 0.05487392018786231, 0.04860478141715638, 0.018248576979006625, -0.004905016845498029, -0.030547681261132508, -0.05714795099327387, -0.0032193038803278273]</t>
+  </si>
+  <si>
+    <t>[1.0, -0.002525254187664789, -0.04395351866747207, -0.09883537232329236, -0.11335429257458329, 0.07431803183308167, 0.025486775210797865, 0.03777172350984037, 0.021905212588827754, -0.012951354087596116, -0.03879417246439179, -0.029310032592469414, -0.0077053457037148335, 0.05671236126776432, 0.054249197375603596, 0.029100293210020035, -0.006396670870171413, -0.03277595465232519, -0.04002549926969663, 0.0029365595332461053]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.000938174311667381</v>
+        <v>0.007093537996962009</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7809438713439286</v>
+        <v>0.7713960392002097</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1183709823931952</v>
+        <v>0.1044958812896311</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1201920800837948</v>
+        <v>-0.1855753646724737</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.7146600096275811</v>
+        <v>0.5381593286732445</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.08437256151599415</v>
+        <v>0.06376423619064685</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.135949515535049</v>
+        <v>0.1782192630903307</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.6457680558412187</v>
+        <v>0.5728745678554105</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.06696972555906473</v>
+        <v>0.06179907510183994</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.0004208491891122551</v>
+        <v>0.001042451192802102</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0003309222042712687</v>
+        <v>0.1127127736981839</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05181414205162736</v>
+        <v>0.04456470552019402</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9470128795253214</v>
+        <v>8.487559062106518E-09</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.001562538384524367</v>
+        <v>-0.001327744496415256</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0003317251781729857</v>
+        <v>0.1122934717130698</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04650875848957307</v>
+        <v>0.008452274866491095</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.946142285572969</v>
+        <v>5.196964653699701E-09</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.0125454530356663</v>
+        <v>0.08014793525174554</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.00319136883951554</v>
+        <v>0.007170031704656806</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.0002683582271512838</v>
+        <v>0.1017035991003381</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04218000568309339</v>
+        <v>1.6376280646107E-11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9502592922823111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.01257965920255122</v>
+        <v>0.05286187043770072</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7871140150637183</v>
+        <v>0.7727068425809218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added risk figure; now fitting on 70% of the length of the time series
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[1.0, 0.020742072449138466, -0.046057578182718904, -0.09987740779527826, -0.11362098275977535, 0.07053872377467447, 0.027242553341174296, 0.038508958376020745, 0.022524839067012383, -0.014046769068594755, -0.041041619122136656, -0.030166978710828258, -0.0071719504665959215, 0.05899539513191117, 0.05611133351917008, 0.03036155380748464, -0.006839678743164695, -0.03382079672006651, -0.04097821460225061, 0.002374139634956119]</t>
+    <t>[1.0, 0.020993214173052173, -0.04176833174737117, -0.10560999193303837, -0.11533516583456446, 0.07035599977997269, 0.026391251168427818, 0.039913619224905376, 0.020689207515053064, -0.01731142237911526, -0.051325861500777385, -0.03442789447122897, 0.0011335207199031814, 0.059519924174354234, 0.056167899344512606, 0.032211846857381946, -0.01283971000304848, -0.031036381260136484, -0.03772868825354034, -0.002959421961216216]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.059786836446393266, 0.008164407218926334, -0.0022021570605025636, -0.00600966558310538, 0.010383753667678432, 0.016637941679735126, -0.02002175112349545, 0.00828413956072075, -0.008164560034633245, 0.012766997876978145, 0.018733138120191988, 0.013428564824778264, 0.029600391644876812, 0.019874002882877304, -4.271655568156782e-05, -0.015510411516043895, -0.007215655497153533, -0.004023081281778683, -0.012554653841117053]</t>
+    <t>[1.0, 0.05936828066251595, 0.01378317064568642, 0.0013389214288225123, -0.00704774752881248, 0.0019225910247095503, 0.010772661747817163, -0.023827857189336794, 0.0032501902115645103, -0.012778729844369953, 0.004055392072017083, 0.014332596877540838, 0.012405963046405833, 0.03059605823726628, 0.029353599051395, 0.0036666200381629196, -0.01638440717766988, -0.005631955863527286, -0.0010197583031796833, -0.011009909056893315]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.0046055459593722405, -0.03433958921631113, -0.09108536610602833, -0.13236200747524696, 0.09214281163745758, 0.05071434479689837, 0.04263232309750947, 0.03213706187886878, 8.049679111961297e-05, -0.053645870199857094, -0.025443903188358093, -0.010255174641980542, 0.05561505926299536, 0.04912782792613663, 0.018314890859462658, -0.0050686743117231165, -0.0302937502907785, -0.05743611288880337, -0.0029958877751506195]</t>
+    <t>[1.0, 0.0035827774405508667, -0.03340950229404528, -0.09611604744631938, -0.12828549937149172, 0.09389995351401186, 0.047924417783650544, 0.040231768982029424, 0.023845263578730742, -0.009572706618660347, -0.057195874014094296, -0.028917465885140933, 0.0006093134134932231, 0.05672645911762163, 0.04550471288916477, 0.019594759359999013, -0.00822015815457666, -0.028157406905283143, -0.05026168883274082, -0.0043637928357312394]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.0029458747712240037, -0.034465194544982605, -0.09075287544891736, -0.13238801623191018, 0.09284870902027942, 0.050533654351551584, 0.041719372478274556, 0.03344411420821392, 0.00010641221794151788, -0.05233931341253185, -0.025471747071868847, -0.01021390984255276, 0.05487392018786231, 0.04860478141715638, 0.018248576979006625, -0.004905016845498029, -0.030547681261132508, -0.05714795099327387, -0.0032193038803278273]</t>
-  </si>
-  <si>
-    <t>[1.0, -0.002525254187664789, -0.04395351866747207, -0.09883537232329236, -0.11335429257458329, 0.07431803183308167, 0.025486775210797865, 0.03777172350984037, 0.021905212588827754, -0.012951354087596116, -0.03879417246439179, -0.029310032592469414, -0.0077053457037148335, 0.05671236126776432, 0.054249197375603596, 0.029100293210020035, -0.006396670870171413, -0.03277595465232519, -0.04002549926969663, 0.0029365595332461053]</t>
+    <t>[1.0, 0.002532115242903328, -0.03374763094583777, -0.09591283751275625, -0.12865656491069777, 0.0943613200162274, 0.04798658597518958, 0.03923494576515497, 0.02460823006793059, -0.010023409121428005, -0.05636285875729877, -0.029063338915024616, 0.0005479569371484508, 0.05645980672459899, 0.04521190515642551, 0.019553193672920893, -0.008112357540072222, -0.02856324722072384, -0.050440185404500223, -0.004607816837164434]</t>
+  </si>
+  <si>
+    <t>[0.9999999999999998, 0.0008215369934537743, -0.04033836938288315, -0.10505544738136322, -0.11536158852912097, 0.07311314602788013, 0.024833604709608496, 0.03913659028049754, 0.02019155537791576, -0.01647136314383136, -0.049363228480920236, -0.03398459019177501, 0.0007680003207134622, 0.057600756789735724, 0.054690747790072644, 0.03141910170917143, -0.012750466758428274, -0.030560715058727473, -0.03727699042133201, -0.0027492667194408847]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.007093537996962009</v>
+        <v>0.008496645711067738</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7713960392002097</v>
+        <v>0.772939363834608</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1044958812896311</v>
+        <v>0.1048964807954936</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8918518518518519</v>
+        <v>0.8847643641058748</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1855753646724737</v>
+        <v>-0.1812764579519923</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.5381593286732445</v>
+        <v>0.5458046833958783</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.06376423619064685</v>
+        <v>0.06305607484792758</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.1782192630903307</v>
+        <v>0.1799868863271274</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.5728745678554105</v>
+        <v>0.5749375572395075</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.06179907510183994</v>
+        <v>0.06303061886141828</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.001042451192802102</v>
+        <v>0.0009873166335556474</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1127127736981839</v>
+        <v>0.1133115976320104</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04456470552019402</v>
+        <v>0.04222293798008307</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>8.487559062106518E-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.001327744496415256</v>
+        <v>-0.0008399168189114137</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1122934717130698</v>
+        <v>0.113002184732998</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.008452274866491095</v>
+        <v>0.01322364626117355</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>5.196964653699701E-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.08014793525174554</v>
+        <v>0.06340350266431082</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.007170031704656806</v>
+        <v>0.008576308576116158</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1017035991003381</v>
+        <v>0.1024876884301354</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>1.6376280646107E-11</v>
+        <v>1.805300617031429E-10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.05286187043770072</v>
+        <v>0.04526849715481648</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7727068425809218</v>
+        <v>0.77383177592694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some settings, in particular: considering 5 days moving average (non-standardized by std), less batches and less episodes but longer
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[1.0, 0.020742072449138466, -0.046057578182718904, -0.09987740779527826, -0.11362098275977535, 0.07053872377467447, 0.027242553341174296, 0.038508958376020745, 0.022524839067012383, -0.014046769068594755, -0.041041619122136656, -0.030166978710828258, -0.0071719504665959215, 0.05899539513191117, 0.05611133351917008, 0.03036155380748464, -0.006839678743164695, -0.03382079672006651, -0.04097821460225061, 0.002374139634956119]</t>
+    <t>[0.9999999999999998, 0.26003763856789847, 0.20602449448478205, 0.1597469691832025, 0.20825986776328745, 0.3866647177859979, 0.21727082136495096, 0.22149372192605693, 0.19520850351139343, 0.1644898527715792, 0.1594244972717661, 0.13889031921796882, 0.19804811655713567, 0.18451236965685267, 0.18617461346997563, 0.17362687256743825, 0.14815905112567532, 0.13262519010195487, 0.15237850217607135, 0.15381158690601096]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.059786836446393266, 0.008164407218926334, -0.0022021570605025636, -0.00600966558310538, 0.010383753667678432, 0.016637941679735126, -0.02002175112349545, 0.00828413956072075, -0.008164560034633245, 0.012766997876978145, 0.018733138120191988, 0.013428564824778264, 0.029600391644876812, 0.019874002882877304, -4.271655568156782e-05, -0.015510411516043895, -0.007215655497153533, -0.004023081281778683, -0.012554653841117053]</t>
+    <t>[1.0, 0.2574247320295584, 0.25225877390737717, 0.21420852687443614, 0.2129895607788758, 0.25274910329965766, 0.18989586675965722, 0.17883538724352283, 0.16787643220697704, 0.1567448687619555, 0.1806829002034267, 0.1526544170395751, 0.18293572393069413, 0.16468814120584158, 0.16681676155815273, 0.1639826028816237, 0.1638623156680472, 0.1604368708196883, 0.17092566112809743, 0.14391953812945438]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.0046055459593722405, -0.03433958921631113, -0.09108536610602833, -0.13236200747524696, 0.09214281163745758, 0.05071434479689837, 0.04263232309750947, 0.03213706187886878, 8.049679111961297e-05, -0.053645870199857094, -0.025443903188358093, -0.010255174641980542, 0.05561505926299536, 0.04912782792613663, 0.018314890859462658, -0.0050686743117231165, -0.0302937502907785, -0.05743611288880337, -0.0029958877751506195]</t>
+    <t>[1.0, 0.008357227091285778, -0.033522811890720365, -0.07715060906364973, -0.07048078881447314, 0.2702364925151802, 0.004314955160213761, 0.04211372372469305, 9.402743801944046e-05, -0.03467394783274602, -0.04626321607775001, -0.06763779991936066, -0.002035940512775672, -0.008138706890245801, 0.01687747015950369, 0.018778925322410527, -0.021237562162973293, -0.04839882685446983, -0.06910436267687978, -0.021792967432692673]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.0029458747712240037, -0.034465194544982605, -0.09075287544891736, -0.13238801623191018, 0.09284870902027942, 0.050533654351551584, 0.041719372478274556, 0.03344411420821392, 0.00010641221794151788, -0.05233931341253185, -0.025471747071868847, -0.01021390984255276, 0.05487392018786231, 0.04860478141715638, 0.018248576979006625, -0.004905016845498029, -0.030547681261132508, -0.05714795099327387, -0.0032193038803278273]</t>
-  </si>
-  <si>
-    <t>[1.0, -0.002525254187664789, -0.04395351866747207, -0.09883537232329236, -0.11335429257458329, 0.07431803183308167, 0.025486775210797865, 0.03777172350984037, 0.021905212588827754, -0.012951354087596116, -0.03879417246439179, -0.029310032592469414, -0.0077053457037148335, 0.05671236126776432, 0.054249197375603596, 0.029100293210020035, -0.006396670870171413, -0.03277595465232519, -0.04002549926969663, 0.0029365595332461053]</t>
+    <t>[1.0, 0.006994302699577481, -0.0343544569674512, -0.07784624053438803, -0.07116840212161608, 0.27013063393374553, 0.0037843186126448104, 0.04147781650032528, -0.0005101822586543604, -0.035030644416461816, -0.04683547178875497, -0.0676438631901248, -0.002343650114997198, -0.008690267521857349, 0.016148648209967458, 0.018186364013949737, -0.021518107935262678, -0.04820059659914482, -0.06932555832395212, -0.021857769567628412]</t>
+  </si>
+  <si>
+    <t>[0.9999999999999998, 0.026910216166365526, -0.01813501093009271, -0.047260640713221856, -0.03339288538954057, 0.2142768596116096, -0.019706406178560662, 0.023322009328276168, -0.0017835395578737025, -0.04504212849192158, -0.03314730519719008, -0.06126497828459132, 0.004449291431843918, -0.00045798308374967735, 0.0051632238047335174, 0.014767889759065029, -0.021590259164887958, -0.04075613801926588, -0.04076433306592119, -0.023396020458887647]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.007093537996962009</v>
+        <v>0.0004844214392533607</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7713960392002097</v>
+        <v>0.7798658526816847</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1044958812896311</v>
+        <v>0.1280320194750863</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.8918518518518519</v>
+        <v>0.908130081300813</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1855753646724737</v>
+        <v>-0.1330743634244479</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.5381593286732445</v>
+        <v>0.7003805508813929</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.06376423619064685</v>
+        <v>0.0893598703809307</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.1782192630903307</v>
+        <v>0.1507729279382539</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.5728745678554105</v>
+        <v>0.629820546979082</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.06179907510183994</v>
+        <v>0.07210868033083918</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.001042451192802102</v>
+        <v>-0.0003018641867290171</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1127127736981839</v>
+        <v>0.001258914372815595</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04456470552019402</v>
+        <v>0.06199770195676332</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>8.487559062106518E-09</v>
+        <v>0.929033465014958</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.001327744496415256</v>
+        <v>-0.001933675721538139</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1122934717130698</v>
+        <v>0.001269239019146223</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.008452274866491095</v>
+        <v>0.0557718394638874</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>5.196964653699701E-09</v>
+        <v>0.9278333736867835</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.08014793525174554</v>
+        <v>0.01501718335146807</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.007170031704656806</v>
+        <v>0.002665281902989896</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1017035991003381</v>
+        <v>0.001010051145472083</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>1.6376280646107E-11</v>
+        <v>0.04647750030145447</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.934875304760624</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.05286187043770072</v>
+        <v>0.02061546307598787</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7727068425809218</v>
+        <v>0.7868578141333236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-set settings and starting testing
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[0.9999999999999998, 0.26003763856789847, 0.20602449448478205, 0.1597469691832025, 0.20825986776328745, 0.3866647177859979, 0.21727082136495096, 0.22149372192605693, 0.19520850351139343, 0.1644898527715792, 0.1594244972717661, 0.13889031921796882, 0.19804811655713567, 0.18451236965685267, 0.18617461346997563, 0.17362687256743825, 0.14815905112567532, 0.13262519010195487, 0.15237850217607135, 0.15381158690601096]</t>
+    <t>[1.0, 0.03591633023658923, -0.03202675534859124, -0.10176320494358693, -0.11019256216814352, 0.07496515225145116, 0.018140790266992772, 0.030603399237779473, 0.011666100456573084, -0.018714686383796822, -0.04237695261679498, -0.03351079806106292, -0.008584719366121306, 0.05106730503852144, 0.04853627039262523, 0.03580689289578694, -0.00538901046711703, -0.03770368103526971, -0.03574853699430846, -0.0042334470341165754]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.2574247320295584, 0.25225877390737717, 0.21420852687443614, 0.2129895607788758, 0.25274910329965766, 0.18989586675965722, 0.17883538724352283, 0.16787643220697704, 0.1567448687619555, 0.1806829002034267, 0.1526544170395751, 0.18293572393069413, 0.16468814120584158, 0.16681676155815273, 0.1639826028816237, 0.1638623156680472, 0.1604368708196883, 0.17092566112809743, 0.14391953812945438]</t>
+    <t>[0.9999999999999998, 0.08479294654618728, 0.01881629546687745, 0.005265668258526909, -0.004825981679042169, 0.001743930812811218, 0.006134634894567925, -0.02707074731679678, 0.00013728442882836723, -0.01613409079524153, 0.008705904118283434, 0.012609553881461523, -0.003237097404894301, 0.025518956925377815, 0.020936588226391134, 0.0002019237245177806, -0.02130525918623366, -0.01751037344892199, -2.416205482189091e-05, -0.018003619111308346]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.008357227091285778, -0.033522811890720365, -0.07715060906364973, -0.07048078881447314, 0.2702364925151802, 0.004314955160213761, 0.04211372372469305, 9.402743801944046e-05, -0.03467394783274602, -0.04626321607775001, -0.06763779991936066, -0.002035940512775672, -0.008138706890245801, 0.01687747015950369, 0.018778925322410527, -0.021237562162973293, -0.04839882685446983, -0.06910436267687978, -0.021792967432692673]</t>
+    <t>[1.0, -0.002267298700155771, -0.028888846210529506, -0.10057383077991917, -0.12177658988596707, 0.09792843714912494, 0.0353070001456782, 0.0399430116107057, 0.015415262220788059, -0.014373956866661741, -0.054595642143399514, -0.02849636875805811, -0.004467030271756254, 0.05169600877879758, 0.038008868427548345, 0.02073322594082356, 0.0009768723167918648, -0.037133387736442036, -0.049227827358005564, -0.010584493127810877]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.006994302699577481, -0.0343544569674512, -0.07784624053438803, -0.07116840212161608, 0.27013063393374553, 0.0037843186126448104, 0.04147781650032528, -0.0005101822586543604, -0.035030644416461816, -0.04683547178875497, -0.0676438631901248, -0.002343650114997198, -0.008690267521857349, 0.016148648209967458, 0.018186364013949737, -0.021518107935262678, -0.04820059659914482, -0.06932555832395212, -0.021857769567628412]</t>
-  </si>
-  <si>
-    <t>[0.9999999999999998, 0.026910216166365526, -0.01813501093009271, -0.047260640713221856, -0.03339288538954057, 0.2142768596116096, -0.019706406178560662, 0.023322009328276168, -0.0017835395578737025, -0.04504212849192158, -0.03314730519719008, -0.06126497828459132, 0.004449291431843918, -0.00045798308374967735, 0.0051632238047335174, 0.014767889759065029, -0.021590259164887958, -0.04075613801926588, -0.04076433306592119, -0.023396020458887647]</t>
+    <t>[0.9999999999999998, -0.0014456543209884585, -0.029892409040372762, -0.10059671877443724, -0.12308192803867783, 0.09797014636914, 0.03582886573049426, 0.03995540255943347, 0.016239788121979654, -0.014453502975154778, -0.05458894249800588, -0.02887284981659763, -0.004567458867819179, 0.05195265317514172, 0.03838938986279587, 0.020493590686416603, 0.0011455914268146234, -0.037926226471186764, -0.04939571790543775, -0.01140523618028735]</t>
+  </si>
+  <si>
+    <t>[1.0, -0.00512539476321441, -0.03429385765695796, -0.10343142142807313, -0.11426245070439539, 0.07830368694206877, 0.015967829928175505, 0.030162640058722677, 0.01153932504129344, -0.01731615938468597, -0.0395013554744115, -0.03134903721579623, -0.008068273968623705, 0.05062079974583103, 0.04581526262333217, 0.03355951469564344, -0.005924246319156136, -0.03715577842559043, -0.03531137514010312, -0.005208636952932974]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.0004844214392533607</v>
+        <v>0.006825207394459255</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7798658526816847</v>
+        <v>0.7740120446426928</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1280320194750863</v>
+        <v>0.1066737348607805</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.908130081300813</v>
+        <v>0.9008186397984886</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1330743634244479</v>
+        <v>-0.1779548845695258</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.7003805508813929</v>
+        <v>0.5618703997551836</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.0893598703809307</v>
+        <v>0.06552252281878544</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.1507729279382539</v>
+        <v>0.1806170955402093</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.629820546979082</v>
+        <v>0.5738797443335716</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.07210868033083918</v>
+        <v>0.0623646825431965</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.0003018641867290171</v>
+        <v>0.001210009391988734</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001258914372815595</v>
+        <v>0.112714886432367</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.06199770195676332</v>
+        <v>0.05963541914630002</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.929033465014958</v>
+        <v>5.989069439454051E-14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.001933675721538139</v>
+        <v>-0.00105386075390126</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001269239019146223</v>
+        <v>0.112623095055708</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.0557718394638874</v>
+        <v>0.02104708133315268</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9278333736867835</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.01501718335146807</v>
+        <v>0.07857961461559494</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.002665281902989896</v>
+        <v>0.007186473657713147</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001010051145472083</v>
+        <v>0.1019441547454095</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04647750030145447</v>
+        <v>0.00235527575045286</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.934875304760624</v>
+        <v>3.911594282837372E-09</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.02061546307598787</v>
+        <v>0.07904812661771926</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7868578141333236</v>
+        <v>0.7748920970977445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refinemenets in plots; again StdMovingAverage; changed neural network parameters; comparison to GP better parametrized
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[1.0, 0.2505353188685017, 0.2070088104677464, 0.16140671412818208, 0.20077759532895936, 0.3982978361298097, 0.21785879747660014, 0.21196092783940826, 0.1898027773322455, 0.16636793440461314, 0.16875316747709537, 0.14626408700640128, 0.18955603931193862, 0.18060096593763408, 0.18949999250704327, 0.17724202918153914, 0.14914152191558894, 0.13345667715620588, 0.15272040506725118, 0.16353734030687517]</t>
+    <t>[1.0, 0.03591633023658923, -0.03202675534859124, -0.10176320494358693, -0.11019256216814352, 0.07496515225145116, 0.018140790266992772, 0.030603399237779473, 0.011666100456573084, -0.018714686383796822, -0.04237695261679498, -0.03351079806106292, -0.008584719366121306, 0.05106730503852144, 0.04853627039262523, 0.03580689289578694, -0.00538901046711703, -0.03770368103526971, -0.03574853699430846, -0.0042334470341165754]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.24788232362328202, 0.2511946617713343, 0.21728816967872017, 0.20795081477873545, 0.2564247832238742, 0.19650141253355632, 0.17967179125752228, 0.17038493607122498, 0.16561474942860357, 0.18641364684488526, 0.16465024152169458, 0.1797511242853914, 0.16064307783176368, 0.16213665194014015, 0.15827317112235517, 0.1632075721257281, 0.15835192559254505, 0.16524687782538058, 0.14445600529099054]</t>
+    <t>[0.9999999999999998, 0.08479294654618728, 0.01881629546687745, 0.005265668258526909, -0.004825981679042169, 0.001743930812811218, 0.006134634894567925, -0.02707074731679678, 0.00013728442882836723, -0.01613409079524153, 0.008705904118283434, 0.012609553881461523, -0.003237097404894301, 0.025518956925377815, 0.020936588226391134, 0.0002019237245177806, -0.02130525918623366, -0.01751037344892199, -2.416205482189091e-05, -0.018003619111308346]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.00420175088094599, -0.029017622674400795, -0.0783631638269784, -0.07385046389781172, 0.2900781446211474, 0.0007028991342478142, 0.03967616975835489, 0.002633672990889935, -0.035143601237185206, -0.03493933283784308, -0.06959460951056623, -0.004443593408788518, 0.0035992339109453147, 0.02325350622172268, 0.02402933255529769, -0.01776286284177971, -0.05357048473546374, -0.06259238879651562, -0.013934934422063462]</t>
+    <t>[1.0, -0.002267298700155771, -0.028888846210529506, -0.10057383077991917, -0.12177658988596707, 0.09792843714912494, 0.0353070001456782, 0.0399430116107057, 0.015415262220788059, -0.014373956866661741, -0.054595642143399514, -0.02849636875805811, -0.004467030271756254, 0.05169600877879758, 0.038008868427548345, 0.02073322594082356, 0.0009768723167918648, -0.037133387736442036, -0.049227827358005564, -0.010584493127810877]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.0029148442985830023, -0.029948615810677294, -0.07922980829439587, -0.07473920769723265, 0.28998149448501076, 0.00027435688620136025, 0.038820686172707584, 0.0018359057894774666, -0.03561130923767125, -0.035756612413976985, -0.06964542173790876, -0.005032276823162368, 0.0029058983184270587, 0.02241449109438609, 0.023342948605504902, -0.01807482430370738, -0.053254934992511174, -0.0626377634415119, -0.013892009005315481]</t>
-  </si>
-  <si>
-    <t>[0.9999999999999998, 0.01731143491860469, -0.009021819588874195, -0.04495704225424116, -0.04227508636129317, 0.22656892726085556, -0.02038331465702374, 0.017900861140770406, -0.006060018526241905, -0.044405958329506744, -0.019099556193685086, -0.052446623823892605, 0.0002372802761895438, 0.003819866031549903, 0.007736566073883774, 0.016823718942061736, -0.02277366661577481, -0.04249207841636404, -0.03498645054650372, -0.016552472955196768]</t>
+    <t>[0.9999999999999998, -0.0014456543209884585, -0.029892409040372762, -0.10059671877443724, -0.12308192803867783, 0.09797014636914, 0.03582886573049426, 0.03995540255943347, 0.016239788121979654, -0.014453502975154778, -0.05458894249800588, -0.02887284981659763, -0.004567458867819179, 0.05195265317514172, 0.03838938986279587, 0.020493590686416603, 0.0011455914268146234, -0.037926226471186764, -0.04939571790543775, -0.01140523618028735]</t>
+  </si>
+  <si>
+    <t>[1.0, -0.00512539476321441, -0.03429385765695796, -0.10343142142807313, -0.11426245070439539, 0.07830368694206877, 0.015967829928175505, 0.030162640058722677, 0.01153932504129344, -0.01731615938468597, -0.0395013554744115, -0.03134903721579623, -0.008068273968623705, 0.05062079974583103, 0.04581526262333217, 0.03355951469564344, -0.005924246319156136, -0.03715577842559043, -0.03531137514010312, -0.005208636952932974]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.0002197522423666586</v>
+        <v>0.006825207394459255</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7800139040307006</v>
+        <v>0.7740120446426928</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1175875511023965</v>
+        <v>0.1066737348607805</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1260290772802757</v>
+        <v>-0.1779548845695258</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.7039927808178692</v>
+        <v>0.5618703997551836</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.0834441946249746</v>
+        <v>0.06552252281878544</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.137569198534594</v>
+        <v>0.1806170955402093</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.643351394295512</v>
+        <v>0.5738797443335716</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.06430986284625408</v>
+        <v>0.0623646825431965</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.000463364014209001</v>
+        <v>0.001210009391988734</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001250586968488332</v>
+        <v>0.112714886432367</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.06281857410544585</v>
+        <v>0.05963541914630002</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9275003942380922</v>
+        <v>5.989069439454051E-14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.002803422354933974</v>
+        <v>-0.00105386075390126</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001240897971319946</v>
+        <v>0.112623095055708</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05259989591106361</v>
+        <v>0.02104708133315268</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9267060177767591</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.02265231079096239</v>
+        <v>0.07857961461559494</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.002534659128032995</v>
+        <v>0.007186473657713147</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001071481403703373</v>
+        <v>0.1019441547454095</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04380155347864951</v>
+        <v>0.00235527575045286</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9307261796143689</v>
+        <v>3.911594282837372E-09</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.03151460786221222</v>
+        <v>0.07904812661771926</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7843674897342773</v>
+        <v>0.7748920970977445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Settings back to qfin22 presentation - recalibration
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[1.0, 0.03591633023658923, -0.03202675534859124, -0.10176320494358693, -0.11019256216814352, 0.07496515225145116, 0.018140790266992772, 0.030603399237779473, 0.011666100456573084, -0.018714686383796822, -0.04237695261679498, -0.03351079806106292, -0.008584719366121306, 0.05106730503852144, 0.04853627039262523, 0.03580689289578694, -0.00538901046711703, -0.03770368103526971, -0.03574853699430846, -0.0042334470341165754]</t>
+    <t>[0.9999999999999999, 0.25053531886850183, 0.2070088104677465, 0.16140671412818225, 0.2007775953289595, 0.39829783612980957, 0.21785879747660017, 0.21196092783940834, 0.18980277733224551, 0.16636793440461314, 0.16875316747709548, 0.14626408700640145, 0.18955603931193868, 0.18060096593763417, 0.18949999250704327, 0.17724202918153925, 0.1491415219155891, 0.13345667715620596, 0.15272040506725137, 0.16353734030687525]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[0.9999999999999998, 0.08479294654618728, 0.01881629546687745, 0.005265668258526909, -0.004825981679042169, 0.001743930812811218, 0.006134634894567925, -0.02707074731679678, 0.00013728442882836723, -0.01613409079524153, 0.008705904118283434, 0.012609553881461523, -0.003237097404894301, 0.025518956925377815, 0.020936588226391134, 0.0002019237245177806, -0.02130525918623366, -0.01751037344892199, -2.416205482189091e-05, -0.018003619111308346]</t>
+    <t>[1.0, 0.24788232362328175, 0.25119466177133426, 0.21728816967872008, 0.20795081477873534, 0.25642478322387396, 0.19650141253355619, 0.17967179125752206, 0.170384936071225, 0.16561474942860355, 0.18641364684488526, 0.16465024152169458, 0.17975112428539128, 0.16064307783176368, 0.16213665194014015, 0.15827317112235512, 0.16320757212572812, 0.15835192559254507, 0.16524687782538058, 0.14445600529099026]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, -0.002267298700155771, -0.028888846210529506, -0.10057383077991917, -0.12177658988596707, 0.09792843714912494, 0.0353070001456782, 0.0399430116107057, 0.015415262220788059, -0.014373956866661741, -0.054595642143399514, -0.02849636875805811, -0.004467030271756254, 0.05169600877879758, 0.038008868427548345, 0.02073322594082356, 0.0009768723167918648, -0.037133387736442036, -0.049227827358005564, -0.010584493127810877]</t>
+    <t>[1.0, 0.004201750216821353, -0.02901762303504444, -0.07836316415634041, -0.07385046429193737, 0.29007814442142926, 0.0007028987521514844, 0.03967616936611137, 0.0026336726550008887, -0.035143601374413413, -0.03493933296735276, -0.06959460947950259, -0.004443593538558104, 0.003599233721223633, 0.023253506164405257, 0.024029332489905315, -0.01776286285349463, -0.0535704846833113, -0.06259238877039287, -0.01393493439041259]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[0.9999999999999998, -0.0014456543209884585, -0.029892409040372762, -0.10059671877443724, -0.12308192803867783, 0.09797014636914, 0.03582886573049426, 0.03995540255943347, 0.016239788121979654, -0.014453502975154778, -0.05458894249800588, -0.02887284981659763, -0.004567458867819179, 0.05195265317514172, 0.03838938986279587, 0.020493590686416603, 0.0011455914268146234, -0.037926226471186764, -0.04939571790543775, -0.01140523618028735]</t>
-  </si>
-  <si>
-    <t>[1.0, -0.00512539476321441, -0.03429385765695796, -0.10343142142807313, -0.11426245070439539, 0.07830368694206877, 0.015967829928175505, 0.030162640058722677, 0.01153932504129344, -0.01731615938468597, -0.0395013554744115, -0.03134903721579623, -0.008068273968623705, 0.05062079974583103, 0.04581526262333217, 0.03355951469564344, -0.005924246319156136, -0.03715577842559043, -0.03531137514010312, -0.005208636952932974]</t>
+    <t>[1.0, 0.002914844080627883, -0.02994861589357286, -0.07922980836185635, -0.07473920778290714, 0.28998149446158655, 0.0002743567606176772, 0.03882068604845218, 0.0018359056840343817, -0.03561130926008774, -0.03575661242165181, -0.06964542166661328, -0.005032276842763942, 0.0029058982549194944, 0.022414491100625874, 0.023342948609641336, -0.018074824292693262, -0.05325493494007477, -0.06263776340128657, -0.01389200897756158]</t>
+  </si>
+  <si>
+    <t>[1.0, 0.017312018758034203, -0.009021291172054724, -0.04495655705498112, -0.042274395089549055, 0.22657016758964318, -0.020382597209890704, 0.017901471982041953, -0.006059452959098886, -0.044405341211522086, -0.019098943552220964, -0.052446148954848185, 0.00023778335427884556, 0.0038200643449998626, 0.007737091260777032, 0.016824270161854497, -0.0227732712133506, -0.04249179335343721, -0.034986202803351095, -0.016552058793695923]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.006825207394459255</v>
+        <v>0.0002197522423666759</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7740120446426928</v>
+        <v>0.7800139040307</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1066737348607805</v>
+        <v>0.1175875511023965</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1779548845695258</v>
+        <v>-0.1260290772802762</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.5618703997551836</v>
+        <v>0.7039927808178683</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.06552252281878544</v>
+        <v>0.08344419462497459</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.1806170955402093</v>
+        <v>0.1375691985345943</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.5738797443335716</v>
+        <v>0.6433513942955118</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.0623646825431965</v>
+        <v>0.06430986284625408</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.001210009391988734</v>
+        <v>-0.0004633644944563182</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.112714886432367</v>
+        <v>0.001250586996403465</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05963541914630002</v>
+        <v>0.06281857483154474</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>5.989069439454051E-14</v>
+        <v>0.9275003932742789</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.00105386075390126</v>
+        <v>-0.002803422635062306</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.112623095055708</v>
+        <v>0.001240897985507922</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.02104708133315268</v>
+        <v>0.0525998961843661</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.9267060174297441</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.07857961461559494</v>
+        <v>0.02265231069234847</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.007186473657713147</v>
+        <v>0.002534223911403063</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1019441547454095</v>
+        <v>0.0010715122280783</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.00235527575045286</v>
+        <v>0.04380106143789499</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>3.911594282837372E-09</v>
+        <v>0.9307266093739496</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.07904812661771926</v>
+        <v>0.03151259845515691</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7748920970977445</v>
+        <v>0.7843683475058039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated lam and kappa
</commit_message>
<xml_diff>
--- a/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
+++ b/data/financial_time_series_data/financial_time_series_calibrations/WTI-riskDriverType-PnL-factor-calibrations.xlsx
@@ -42,7 +42,7 @@
     <t>abs_epsi_autocorr</t>
   </si>
   <si>
-    <t>[1.0, 0.2505353188685017, 0.2070088104677464, 0.16140671412818208, 0.20077759532895936, 0.3982978361298097, 0.21785879747660014, 0.21196092783940826, 0.1898027773322455, 0.16636793440461314, 0.16875316747709537, 0.14626408700640128, 0.18955603931193862, 0.18060096593763408, 0.18949999250704327, 0.17724202918153914, 0.14914152191558894, 0.13345667715620588, 0.15272040506725118, 0.16353734030687517]</t>
+    <t>[0.9999999999999999, 0.25053531886850183, 0.2070088104677465, 0.16140671412818225, 0.2007775953289595, 0.39829783612980957, 0.21785879747660017, 0.21196092783940834, 0.18980277733224551, 0.16636793440461314, 0.16875316747709548, 0.14626408700640145, 0.18955603931193868, 0.18060096593763417, 0.18949999250704327, 0.17724202918153925, 0.1491415219155891, 0.13345667715620596, 0.15272040506725137, 0.16353734030687525]</t>
   </si>
   <si>
     <t>c</t>
@@ -69,7 +69,7 @@
     <t>sig2_1</t>
   </si>
   <si>
-    <t>[1.0, 0.24788232362328202, 0.2511946617713343, 0.21728816967872017, 0.20795081477873545, 0.2564247832238742, 0.19650141253355632, 0.17967179125752228, 0.17038493607122498, 0.16561474942860357, 0.18641364684488526, 0.16465024152169458, 0.1797511242853914, 0.16064307783176368, 0.16213665194014015, 0.15827317112235517, 0.1632075721257281, 0.15835192559254505, 0.16524687782538058, 0.14445600529099054]</t>
+    <t>[1.0, 0.24788232362328175, 0.25119466177133426, 0.21728816967872008, 0.20795081477873534, 0.25642478322387396, 0.19650141253355619, 0.17967179125752206, 0.170384936071225, 0.16561474942860355, 0.18641364684488526, 0.16465024152169458, 0.17975112428539128, 0.16064307783176368, 0.16213665194014015, 0.15827317112235512, 0.16320757212572812, 0.15835192559254507, 0.16524687782538058, 0.14445600529099026]</t>
   </si>
   <si>
     <t>omega</t>
@@ -81,16 +81,16 @@
     <t>beta</t>
   </si>
   <si>
-    <t>[1.0, 0.00420175088094599, -0.029017622674400795, -0.0783631638269784, -0.07385046389781172, 0.2900781446211474, 0.0007028991342478142, 0.03967616975835489, 0.002633672990889935, -0.035143601237185206, -0.03493933283784308, -0.06959460951056623, -0.004443593408788518, 0.0035992339109453147, 0.02325350622172268, 0.02402933255529769, -0.01776286284177971, -0.05357048473546374, -0.06259238879651562, -0.013934934422063462]</t>
+    <t>[1.0, 0.004201750216821353, -0.02901762303504444, -0.07836316415634041, -0.07385046429193737, 0.29007814442142926, 0.0007028987521514844, 0.03967616936611137, 0.0026336726550008887, -0.035143601374413413, -0.03493933296735276, -0.06959460947950259, -0.004443593538558104, 0.003599233721223633, 0.023253506164405257, 0.024029332489905315, -0.01776286285349463, -0.0535704846833113, -0.06259238877039287, -0.01393493439041259]</t>
   </si>
   <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>[1.0, 0.0029148442985830023, -0.029948615810677294, -0.07922980829439587, -0.07473920769723265, 0.28998149448501076, 0.00027435688620136025, 0.038820686172707584, 0.0018359057894774666, -0.03561130923767125, -0.035756612413976985, -0.06964542173790876, -0.005032276823162368, 0.0029058983184270587, 0.02241449109438609, 0.023342948605504902, -0.01807482430370738, -0.053254934992511174, -0.0626377634415119, -0.013892009005315481]</t>
-  </si>
-  <si>
-    <t>[0.9999999999999998, 0.01731143491860469, -0.009021819588874195, -0.04495704225424116, -0.04227508636129317, 0.22656892726085556, -0.02038331465702374, 0.017900861140770406, -0.006060018526241905, -0.044405958329506744, -0.019099556193685086, -0.052446623823892605, 0.0002372802761895438, 0.003819866031549903, 0.007736566073883774, 0.016823718942061736, -0.02277366661577481, -0.04249207841636404, -0.03498645054650372, -0.016552472955196768]</t>
+    <t>[1.0, 0.002914844080627883, -0.02994861589357286, -0.07922980836185635, -0.07473920778290714, 0.28998149446158655, 0.0002743567606176772, 0.03882068604845218, 0.0018359056840343817, -0.03561130926008774, -0.03575661242165181, -0.06964542166661328, -0.005032276842763942, 0.0029058982549194944, 0.022414491100625874, 0.023342948609641336, -0.018074824292693262, -0.05325493494007477, -0.06263776340128657, -0.01389200897756158]</t>
+  </si>
+  <si>
+    <t>[1.0, 0.017312018758034203, -0.009021291172054724, -0.04495655705498112, -0.042274395089549055, 0.22657016758964318, -0.020382597209890704, 0.017901471982041953, -0.006059452959098886, -0.044405341211522086, -0.019098943552220964, -0.052446148954848185, 0.00023778335427884556, 0.0038200643449998626, 0.007737091260777032, 0.016824270161854497, -0.0227732712133506, -0.04249179335343721, -0.034986202803351095, -0.016552058793695923]</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.0002197522423666586</v>
+        <v>0.0002197522423666759</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.7800139040307006</v>
+        <v>0.7800139040307</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>-0.1260290772802757</v>
+        <v>-0.1260290772802762</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.7039927808178692</v>
+        <v>0.7039927808178683</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.0834441946249746</v>
+        <v>0.08344419462497459</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.137569198534594</v>
+        <v>0.1375691985345943</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.643351394295512</v>
+        <v>0.6433513942955118</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.000463364014209001</v>
+        <v>-0.0004633644944563182</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001250586968488332</v>
+        <v>0.001250586996403465</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -643,7 +643,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.06281857410544585</v>
+        <v>0.06281857483154474</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -651,7 +651,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9275003942380922</v>
+        <v>0.9275003932742789</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.002803422354933974</v>
+        <v>-0.002803422635062306</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -693,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001240897971319946</v>
+        <v>0.001240897985507922</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -701,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.05259989591106361</v>
+        <v>0.0525998961843661</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -709,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9267060177767591</v>
+        <v>0.9267060174297441</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.02265231079096239</v>
+        <v>0.02265231069234847</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.002534659128032995</v>
+        <v>0.002534223911403063</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.001071481403703373</v>
+        <v>0.0010715122280783</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -775,7 +775,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.04380155347864951</v>
+        <v>0.04380106143789499</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9307261796143689</v>
+        <v>0.9307266093739496</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.03151460786221222</v>
+        <v>0.03151259845515691</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.7843674897342773</v>
+        <v>0.7843683475058039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>